<commit_message>
Data phraser used absoulte path rather then realtive
</commit_message>
<xml_diff>
--- a/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
@@ -926,11 +926,11 @@
   </borders>
   <cellStyleXfs count="6">
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="111">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -1267,11 +1267,11 @@
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="6" name="Comma [0]" xfId="0"/>
-    <cellStyle builtinId="0" name="Normal" xfId="1"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="5" name="Percent" xfId="4"/>
-    <cellStyle builtinId="3" name="Comma" xfId="5"/>
+    <cellStyle builtinId="5" name="Percent" xfId="1"/>
+    <cellStyle builtinId="4" name="Currency" xfId="2"/>
+    <cellStyle builtinId="3" name="Comma" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="0" name="Normal" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>

</xml_diff>

<commit_message>
Update data input manager to automcailly create DB if it dones not exist and added all data into new data folder
</commit_message>
<xml_diff>
--- a/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
@@ -926,11 +926,11 @@
   </borders>
   <cellStyleXfs count="6">
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="111">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -1266,12 +1266,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="6" name="Comma [0]" xfId="0"/>
-    <cellStyle builtinId="5" name="Percent" xfId="1"/>
-    <cellStyle builtinId="4" name="Currency" xfId="2"/>
-    <cellStyle builtinId="3" name="Comma" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="0" name="Normal" xfId="5"/>
+    <cellStyle builtinId="3" name="Comma" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="1"/>
+    <cellStyle builtinId="5" name="Percent" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="4"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>

</xml_diff>

<commit_message>
Close db connection in creation of initial db
</commit_message>
<xml_diff>
--- a/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
@@ -926,11 +926,11 @@
   </borders>
   <cellStyleXfs count="6">
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="111">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -1266,12 +1266,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="3" name="Comma" xfId="0"/>
-    <cellStyle builtinId="0" name="Normal" xfId="1"/>
-    <cellStyle builtinId="5" name="Percent" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="4"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="5"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="0"/>
+    <cellStyle builtinId="4" name="Currency" xfId="1"/>
+    <cellStyle builtinId="3" name="Comma" xfId="2"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="3"/>
+    <cellStyle builtinId="5" name="Percent" xfId="4"/>
+    <cellStyle builtinId="0" name="Normal" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -1622,7 +1622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -2383,12 +2383,12 @@
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
   <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -3106,12 +3106,12 @@
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
   <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -3817,12 +3817,12 @@
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
   <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
@@ -5177,6 +5177,6 @@
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins bottom="0.75" footer="0.511805555555555" header="0.511805555555555" left="0.7" right="0.7" top="0.75"/>
   <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="0" verticalDpi="300"/>
-  <legacyDrawing r:id="anysvml"/>
+  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sepearte out table creation from main script :
</commit_message>
<xml_diff>
--- a/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
@@ -929,8 +929,8 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="111">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -1266,12 +1266,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="6" name="Comma [0]" xfId="0"/>
-    <cellStyle builtinId="4" name="Currency" xfId="1"/>
-    <cellStyle builtinId="3" name="Comma" xfId="2"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="3"/>
-    <cellStyle builtinId="5" name="Percent" xfId="4"/>
-    <cellStyle builtinId="0" name="Normal" xfId="5"/>
+    <cellStyle builtinId="3" name="Comma" xfId="0"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="0" name="Normal" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>

</xml_diff>

<commit_message>
No db select for connection
</commit_message>
<xml_diff>
--- a/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
@@ -925,11 +925,11 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="111">
@@ -1266,12 +1266,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="3" name="Comma" xfId="0"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="0" name="Normal" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="1"/>
+    <cellStyle builtinId="5" name="Percent" xfId="2"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="3"/>
+    <cellStyle builtinId="3" name="Comma" xfId="4"/>
+    <cellStyle builtinId="4" name="Currency" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>

</xml_diff>

<commit_message>
using new library to build database
</commit_message>
<xml_diff>
--- a/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/server/Csi42001Vm1ServerFiles/src/main/resources/static/helpers/data_cleaning/data_storage/new_data/B0.02 B0.03 B0.04 Timetable.xlsx
@@ -925,8 +925,8 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
@@ -1266,12 +1266,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="1"/>
-    <cellStyle builtinId="5" name="Percent" xfId="2"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="3"/>
-    <cellStyle builtinId="3" name="Comma" xfId="4"/>
-    <cellStyle builtinId="4" name="Currency" xfId="5"/>
+    <cellStyle builtinId="4" name="Currency" xfId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="1"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="2"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="3"/>
+    <cellStyle builtinId="5" name="Percent" xfId="4"/>
+    <cellStyle builtinId="3" name="Comma" xfId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>

</xml_diff>